<commit_message>
update draft_mini_app, add file word report and update compare many model CNN train pose
</commit_message>
<xml_diff>
--- a/tracking_train_luanvan.xlsx
+++ b/tracking_train_luanvan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000EB08E-798B-4D11-B697-10A66B0C19DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E264BE-30B9-4999-ADA3-12DF5E419788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EB51D8B-8C57-402C-8EC1-49E82BB5862F}"/>
   </bookViews>
@@ -390,78 +390,105 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -469,33 +496,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952FB45B-156D-4D83-BAD6-97DE485FBD1A}">
   <dimension ref="A2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -834,53 +834,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="19" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="25" t="s">
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -912,46 +912,46 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="32"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -1114,106 +1114,106 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="19" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="25" t="s">
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="26"/>
-      <c r="J19" s="27"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="30"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="37" t="s">
+      <c r="I21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="38" t="s">
+      <c r="J21" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="41"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="16"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="44"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
@@ -1377,36 +1377,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="E3:G4"/>
+    <mergeCell ref="H3:J4"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:D20"/>
+    <mergeCell ref="E19:G20"/>
+    <mergeCell ref="H19:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="C21:C23"/>
     <mergeCell ref="E21:E23"/>
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="H21:H23"/>
     <mergeCell ref="I21:I23"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="A18:J18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:D20"/>
-    <mergeCell ref="E19:G20"/>
-    <mergeCell ref="H19:J20"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="E3:G4"/>
-    <mergeCell ref="H3:J4"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update train detect sleep with RandomForest
</commit_message>
<xml_diff>
--- a/tracking_train_luanvan.xlsx
+++ b/tracking_train_luanvan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E264BE-30B9-4999-ADA3-12DF5E419788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C114CEC-5CE0-4628-A17E-80A006A39F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EB51D8B-8C57-402C-8EC1-49E82BB5862F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>Accuracy</t>
   </si>
@@ -145,6 +145,39 @@
   </si>
   <si>
     <t>0.110</t>
+  </si>
+  <si>
+    <t>RandomForest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_ESTIMATORS =  100             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_ESTIMATORS =  250 </t>
+  </si>
+  <si>
+    <t>N_ESTIMATORS =  450</t>
+  </si>
+  <si>
+    <t>Max_Depth = 15</t>
+  </si>
+  <si>
+    <t>Max_Depth = 55</t>
+  </si>
+  <si>
+    <t>Max_Depth = 75</t>
+  </si>
+  <si>
+    <t>8.98</t>
+  </si>
+  <si>
+    <t>98.0</t>
+  </si>
+  <si>
+    <t>98.5</t>
+  </si>
+  <si>
+    <t>97.6</t>
   </si>
 </sst>
 </file>
@@ -366,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -390,6 +423,96 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -408,95 +531,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952FB45B-156D-4D83-BAD6-97DE485FBD1A}">
-  <dimension ref="A2:J28"/>
+  <dimension ref="A2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -834,53 +873,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="27" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="33" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="34"/>
-      <c r="J3" s="35"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="35"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -912,46 +951,46 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="41" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="42" t="s">
+      <c r="F6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="40"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -1114,106 +1153,106 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="27" t="s">
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="33" t="s">
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="35"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="38"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="35"/>
     </row>
     <row r="21" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I21" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="J21" s="36" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="16"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="37"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="17"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
@@ -1375,28 +1414,336 @@
         <v>39</v>
       </c>
     </row>
+    <row r="33" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="25"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="31"/>
+      <c r="J34" s="32"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="35"/>
+    </row>
+    <row r="36" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="H36" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="I36" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="J36" s="36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="46"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="37"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="46"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="38"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="46"/>
+      <c r="B39" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="I39" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J39" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="46"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="37"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="2">
+        <v>98121</v>
+      </c>
+      <c r="C41" s="2">
+        <v>96606</v>
+      </c>
+      <c r="D41" s="2">
+        <v>96666</v>
+      </c>
+      <c r="E41" s="3">
+        <v>97583</v>
+      </c>
+      <c r="F41" s="3">
+        <v>97416</v>
+      </c>
+      <c r="G41" s="3">
+        <v>98333</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2">
+        <v>98088</v>
+      </c>
+      <c r="C42" s="2">
+        <v>96507</v>
+      </c>
+      <c r="D42" s="2">
+        <v>96584</v>
+      </c>
+      <c r="E42" s="3">
+        <v>97489</v>
+      </c>
+      <c r="F42" s="3">
+        <v>97330</v>
+      </c>
+      <c r="G42" s="3">
+        <v>98287</v>
+      </c>
+      <c r="H42" s="4">
+        <v>97846</v>
+      </c>
+      <c r="I42" s="4">
+        <v>98341</v>
+      </c>
+      <c r="J42" s="4">
+        <v>97496</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="2">
+        <v>98080</v>
+      </c>
+      <c r="C43" s="2">
+        <v>96660</v>
+      </c>
+      <c r="D43" s="2">
+        <v>96724</v>
+      </c>
+      <c r="E43" s="3">
+        <v>97666</v>
+      </c>
+      <c r="F43" s="3">
+        <v>97509</v>
+      </c>
+      <c r="G43" s="3">
+        <v>98396</v>
+      </c>
+      <c r="H43" s="4">
+        <v>97843</v>
+      </c>
+      <c r="I43" s="4">
+        <v>98488</v>
+      </c>
+      <c r="J43" s="4">
+        <v>97471</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="2">
+        <v>98204</v>
+      </c>
+      <c r="C44" s="2">
+        <v>96668</v>
+      </c>
+      <c r="D44" s="2">
+        <v>96632</v>
+      </c>
+      <c r="E44" s="3">
+        <v>97587</v>
+      </c>
+      <c r="F44" s="3">
+        <v>97431</v>
+      </c>
+      <c r="G44" s="3">
+        <v>98347</v>
+      </c>
+      <c r="H44" s="4">
+        <v>98172</v>
+      </c>
+      <c r="I44" s="4">
+        <v>98390</v>
+      </c>
+      <c r="J44" s="4">
+        <v>97876</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="2">
+        <v>19683</v>
+      </c>
+      <c r="D45" s="2">
+        <v>34112</v>
+      </c>
+      <c r="E45" s="3">
+        <v>7494</v>
+      </c>
+      <c r="F45" s="3">
+        <v>17760</v>
+      </c>
+      <c r="G45" s="3">
+        <v>32569</v>
+      </c>
+      <c r="H45" s="4">
+        <v>7027</v>
+      </c>
+      <c r="I45" s="4">
+        <v>16923</v>
+      </c>
+      <c r="J45" s="4">
+        <v>30551</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="E3:G4"/>
-    <mergeCell ref="H3:J4"/>
-    <mergeCell ref="A18:J18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:D20"/>
-    <mergeCell ref="E19:G20"/>
-    <mergeCell ref="H19:J20"/>
+  <mergeCells count="54">
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="I36:I38"/>
+    <mergeCell ref="J36:J38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:D35"/>
+    <mergeCell ref="E34:G35"/>
+    <mergeCell ref="H34:J35"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="B21:B23"/>
@@ -1407,6 +1754,26 @@
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="H21:H23"/>
     <mergeCell ref="I21:I23"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:D20"/>
+    <mergeCell ref="E19:G20"/>
+    <mergeCell ref="H19:J20"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="E3:G4"/>
+    <mergeCell ref="H3:J4"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add new file, and update file
</commit_message>
<xml_diff>
--- a/tracking_train_luanvan.xlsx
+++ b/tracking_train_luanvan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C114CEC-5CE0-4628-A17E-80A006A39F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0B7DC2-4E9B-49BD-835F-275625A346F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EB51D8B-8C57-402C-8EC1-49E82BB5862F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="59">
   <si>
     <t>Accuracy</t>
   </si>
@@ -42,9 +42,6 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>SVC</t>
-  </si>
-  <si>
     <t>Kfold = 50, Avg = 50</t>
   </si>
   <si>
@@ -178,13 +175,40 @@
   </si>
   <si>
     <t>97.6</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>Epoch = 20</t>
+  </si>
+  <si>
+    <t>Epoch = 50</t>
+  </si>
+  <si>
+    <t>Epoch = 70</t>
+  </si>
+  <si>
+    <t>BS = 24</t>
+  </si>
+  <si>
+    <t>BS = 64</t>
+  </si>
+  <si>
+    <t>BS = 128</t>
+  </si>
+  <si>
+    <t>TIME (sec)</t>
+  </si>
+  <si>
+    <t>SVM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +240,24 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,8 +312,74 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAE3F3"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFDAE3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7F7F7F"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -395,11 +501,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -423,6 +566,36 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,8 +707,107 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952FB45B-156D-4D83-BAD6-97DE485FBD1A}">
-  <dimension ref="A2:J45"/>
+  <dimension ref="A2:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -873,124 +1145,124 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="18" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="24" t="s">
+      <c r="F3" s="35"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="30" t="s">
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+    </row>
+    <row r="4" spans="1:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="45"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="32"/>
-    </row>
-    <row r="4" spans="1:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="35"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="D6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="F6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="H6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="I6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="13"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -999,29 +1271,29 @@
       <c r="B8" s="2">
         <v>97393</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="16">
         <v>97515</v>
       </c>
       <c r="D8" s="2">
         <v>96969</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="3">
+        <v>16</v>
+      </c>
+      <c r="F8" s="16">
         <v>98916</v>
       </c>
       <c r="G8" s="3">
         <v>97500</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>18</v>
+      <c r="H8" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1031,7 +1303,7 @@
       <c r="B9" s="2">
         <v>97296</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="16">
         <v>97432</v>
       </c>
       <c r="D9" s="2">
@@ -1040,13 +1312,13 @@
       <c r="E9" s="3">
         <v>97413</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="16">
         <v>98859</v>
       </c>
       <c r="G9" s="3">
         <v>97357</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="16">
         <v>98134</v>
       </c>
       <c r="I9" s="4">
@@ -1063,7 +1335,7 @@
       <c r="B10" s="2">
         <v>97313</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="16">
         <v>97547</v>
       </c>
       <c r="D10" s="2">
@@ -1072,13 +1344,13 @@
       <c r="E10" s="3">
         <v>97425</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="16">
         <v>98876</v>
       </c>
       <c r="G10" s="3">
         <v>97625</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="16">
         <v>98256</v>
       </c>
       <c r="I10" s="4">
@@ -1095,7 +1367,7 @@
       <c r="B11" s="2">
         <v>97433</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="16">
         <v>97441</v>
       </c>
       <c r="D11" s="2">
@@ -1104,13 +1376,13 @@
       <c r="E11" s="3">
         <v>97605</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="16">
         <v>99001</v>
       </c>
       <c r="G11" s="3">
         <v>97306</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="16">
         <v>98221</v>
       </c>
       <c r="I11" s="4">
@@ -1127,7 +1399,7 @@
       <c r="B12" s="2">
         <v>10624</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="16">
         <v>1784</v>
       </c>
       <c r="D12" s="2">
@@ -1136,123 +1408,123 @@
       <c r="E12" s="3">
         <v>4798</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>19</v>
+      <c r="F12" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="4">
+        <v>21</v>
+      </c>
+      <c r="H12" s="16">
         <v>3004</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="B19" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="35"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="41"/>
+      <c r="J19" s="42"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="19"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="45"/>
+    </row>
+    <row r="21" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="32"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="35"/>
-    </row>
-    <row r="21" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="39" t="s">
+      <c r="C21" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="D21" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="G21" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="39" t="s">
+      <c r="H21" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="42" t="s">
+      <c r="J21" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="36" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="22" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="37"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="47"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="38"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="48"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
@@ -1261,14 +1533,14 @@
       <c r="B24" s="2">
         <v>96060</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="16">
         <v>96606</v>
       </c>
       <c r="D24" s="2">
         <v>95636</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>31</v>
+      <c r="E24" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="F24" s="3">
         <v>96166</v>
@@ -1277,13 +1549,13 @@
         <v>96083</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1293,13 +1565,13 @@
       <c r="B25" s="2">
         <v>95958</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="16">
         <v>96471</v>
       </c>
       <c r="D25" s="2">
         <v>95464</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="16">
         <v>96310</v>
       </c>
       <c r="F25" s="3">
@@ -1311,7 +1583,7 @@
       <c r="H25" s="4">
         <v>95871</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="16">
         <v>96067</v>
       </c>
       <c r="J25" s="4">
@@ -1325,13 +1597,13 @@
       <c r="B26" s="2">
         <v>96064</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="16">
         <v>96554</v>
       </c>
       <c r="D26" s="2">
         <v>95740</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="16">
         <v>96371</v>
       </c>
       <c r="F26" s="3">
@@ -1343,7 +1615,7 @@
       <c r="H26" s="4">
         <v>96066</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="16">
         <v>96346</v>
       </c>
       <c r="J26" s="4">
@@ -1357,13 +1629,13 @@
       <c r="B27" s="2">
         <v>96218</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="16">
         <v>96667</v>
       </c>
       <c r="D27" s="2">
         <v>95545</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="16">
         <v>96773</v>
       </c>
       <c r="F27" s="3">
@@ -1375,7 +1647,7 @@
       <c r="H27" s="4">
         <v>96184</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="16">
         <v>96273</v>
       </c>
       <c r="J27" s="4">
@@ -1389,180 +1661,180 @@
       <c r="B28" s="2">
         <v>1337</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="H28" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="4" t="s">
+    </row>
+    <row r="33" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+      <c r="B34" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="41"/>
+      <c r="J34" s="42"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="19"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="45"/>
+    </row>
+    <row r="36" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I34" s="31"/>
-      <c r="J34" s="32"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="35"/>
-    </row>
-    <row r="36" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="39" t="s">
+      <c r="C36" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="D36" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="36" t="s">
+      <c r="E36" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="G36" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="I36" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="J36" s="46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="56"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="47"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="56"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="48"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="56"/>
+      <c r="B39" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="F36" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="36" t="s">
+      <c r="C39" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="H36" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="I36" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" s="36" t="s">
+      <c r="F39" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="H39" s="49" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="37"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="46"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="38"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="46"/>
-      <c r="B39" s="39" t="s">
+      <c r="I39" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="42" t="s">
+      <c r="J39" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E39" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="G39" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H39" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="I39" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="J39" s="36" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="40" spans="1:10" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="46"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="37"/>
+      <c r="A40" s="56"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="47"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="16">
         <v>98121</v>
       </c>
       <c r="C41" s="2">
@@ -1577,24 +1849,24 @@
       <c r="F41" s="3">
         <v>97416</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="16">
         <v>98333</v>
       </c>
       <c r="H41" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I41" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="16">
         <v>98088</v>
       </c>
       <c r="C42" s="2">
@@ -1609,13 +1881,13 @@
       <c r="F42" s="3">
         <v>97330</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="16">
         <v>98287</v>
       </c>
       <c r="H42" s="4">
         <v>97846</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42" s="16">
         <v>98341</v>
       </c>
       <c r="J42" s="4">
@@ -1626,7 +1898,7 @@
       <c r="A43" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="16">
         <v>98080</v>
       </c>
       <c r="C43" s="2">
@@ -1641,13 +1913,13 @@
       <c r="F43" s="3">
         <v>97509</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="16">
         <v>98396</v>
       </c>
       <c r="H43" s="4">
         <v>97843</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="16">
         <v>98488</v>
       </c>
       <c r="J43" s="4">
@@ -1658,7 +1930,7 @@
       <c r="A44" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="16">
         <v>98204</v>
       </c>
       <c r="C44" s="2">
@@ -1673,13 +1945,13 @@
       <c r="F44" s="3">
         <v>97431</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="16">
         <v>98347</v>
       </c>
       <c r="H44" s="4">
         <v>98172</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44" s="16">
         <v>98390</v>
       </c>
       <c r="J44" s="4">
@@ -1690,8 +1962,8 @@
       <c r="A45" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>47</v>
+      <c r="B45" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="C45" s="2">
         <v>19683</v>
@@ -1705,21 +1977,328 @@
       <c r="F45" s="3">
         <v>17760</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="16">
         <v>32569</v>
       </c>
       <c r="H45" s="4">
         <v>7027</v>
       </c>
-      <c r="I45" s="4">
+      <c r="I45" s="16">
         <v>16923</v>
       </c>
       <c r="J45" s="4">
         <v>30551</v>
       </c>
     </row>
+    <row r="49" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="58"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="59"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="63"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="69"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" s="75"/>
+      <c r="J50" s="76"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="61"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="72"/>
+      <c r="G51" s="73"/>
+      <c r="H51" s="77"/>
+      <c r="I51" s="78"/>
+      <c r="J51" s="79"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="84" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="E52" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" s="84" t="s">
+        <v>52</v>
+      </c>
+      <c r="G52" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="H52" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="I52" s="84" t="s">
+        <v>52</v>
+      </c>
+      <c r="J52" s="87" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="80"/>
+      <c r="B53" s="82"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="88"/>
+      <c r="E53" s="82"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="88"/>
+      <c r="H53" s="82"/>
+      <c r="I53" s="85"/>
+      <c r="J53" s="88"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="80"/>
+      <c r="B54" s="83"/>
+      <c r="C54" s="86"/>
+      <c r="D54" s="89"/>
+      <c r="E54" s="83"/>
+      <c r="F54" s="86"/>
+      <c r="G54" s="89"/>
+      <c r="H54" s="83"/>
+      <c r="I54" s="86"/>
+      <c r="J54" s="89"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="61"/>
+      <c r="B55" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J55" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="13">
+        <v>96602</v>
+      </c>
+      <c r="C56" s="13">
+        <v>96759</v>
+      </c>
+      <c r="D56" s="17">
+        <v>96795</v>
+      </c>
+      <c r="E56" s="14">
+        <v>97129</v>
+      </c>
+      <c r="F56" s="14">
+        <v>97193</v>
+      </c>
+      <c r="G56" s="18">
+        <v>97274</v>
+      </c>
+      <c r="H56" s="15">
+        <v>97191</v>
+      </c>
+      <c r="I56" s="17">
+        <v>97717</v>
+      </c>
+      <c r="J56" s="15">
+        <v>97434</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="13">
+        <v>96568</v>
+      </c>
+      <c r="C57" s="13">
+        <v>96847</v>
+      </c>
+      <c r="D57" s="17">
+        <v>96819</v>
+      </c>
+      <c r="E57" s="14">
+        <v>97153</v>
+      </c>
+      <c r="F57" s="14">
+        <v>97274</v>
+      </c>
+      <c r="G57" s="18">
+        <v>97337</v>
+      </c>
+      <c r="H57" s="15">
+        <v>97264</v>
+      </c>
+      <c r="I57" s="17">
+        <v>97722</v>
+      </c>
+      <c r="J57" s="15">
+        <v>97494</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="13">
+        <v>97393</v>
+      </c>
+      <c r="C58" s="13">
+        <v>97524</v>
+      </c>
+      <c r="D58" s="17">
+        <v>97490</v>
+      </c>
+      <c r="E58" s="14">
+        <v>97824</v>
+      </c>
+      <c r="F58" s="14">
+        <v>97954</v>
+      </c>
+      <c r="G58" s="18">
+        <v>98131</v>
+      </c>
+      <c r="H58" s="15">
+        <v>98596</v>
+      </c>
+      <c r="I58" s="17">
+        <v>98625</v>
+      </c>
+      <c r="J58" s="15">
+        <v>98335</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="13">
+        <v>95812</v>
+      </c>
+      <c r="C59" s="13">
+        <v>96227</v>
+      </c>
+      <c r="D59" s="17">
+        <v>96188</v>
+      </c>
+      <c r="E59" s="14">
+        <v>96557</v>
+      </c>
+      <c r="F59" s="14">
+        <v>96647</v>
+      </c>
+      <c r="G59" s="18">
+        <v>96605</v>
+      </c>
+      <c r="H59" s="15">
+        <v>96008</v>
+      </c>
+      <c r="I59" s="17">
+        <v>96889</v>
+      </c>
+      <c r="J59" s="15">
+        <v>96724</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="13">
+        <v>183929</v>
+      </c>
+      <c r="C60" s="13">
+        <v>254667</v>
+      </c>
+      <c r="D60" s="17">
+        <v>276158</v>
+      </c>
+      <c r="E60" s="14">
+        <v>165595</v>
+      </c>
+      <c r="F60" s="14">
+        <v>233255</v>
+      </c>
+      <c r="G60" s="18">
+        <v>246635</v>
+      </c>
+      <c r="H60" s="15">
+        <v>140410</v>
+      </c>
+      <c r="I60" s="17">
+        <v>215629</v>
+      </c>
+      <c r="J60" s="15">
+        <v>268728</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="69">
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="H52:H54"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="J52:J54"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:D51"/>
+    <mergeCell ref="E50:G51"/>
+    <mergeCell ref="H50:J51"/>
     <mergeCell ref="G39:G40"/>
     <mergeCell ref="H39:H40"/>
     <mergeCell ref="I39:I40"/>

</xml_diff>

<commit_message>
add file report v5
</commit_message>
<xml_diff>
--- a/tracking_train_luanvan.xlsx
+++ b/tracking_train_luanvan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0B7DC2-4E9B-49BD-835F-275625A346F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CBDFC1-2219-4D8C-868B-FCE580E79C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EB51D8B-8C57-402C-8EC1-49E82BB5862F}"/>
   </bookViews>
@@ -208,7 +208,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,14 +233,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -257,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,44 +270,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
     <fill>
@@ -338,44 +294,104 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA9D18E"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFD0CECE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7F7F7F"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFD0CECE"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
   </fills>
@@ -542,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -551,263 +567,344 @@
     <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="1" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1125,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952FB45B-156D-4D83-BAD6-97DE485FBD1A}">
   <dimension ref="A2:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -1145,133 +1242,133 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
     </row>
     <row r="3" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="34" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="40" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="49" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="51" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="23"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="2">
         <v>97393</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="32">
         <v>97515</v>
       </c>
       <c r="D8" s="2">
@@ -1280,30 +1377,30 @@
       <c r="E8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="32">
         <v>98916</v>
       </c>
       <c r="G8" s="3">
         <v>97500</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="53" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="2">
         <v>97296</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="32">
         <v>97432</v>
       </c>
       <c r="D9" s="2">
@@ -1312,30 +1409,30 @@
       <c r="E9" s="3">
         <v>97413</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="32">
         <v>98859</v>
       </c>
       <c r="G9" s="3">
         <v>97357</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="32">
         <v>98134</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="53">
         <v>97183</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="53">
         <v>98034</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="2">
         <v>97313</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="32">
         <v>97547</v>
       </c>
       <c r="D10" s="2">
@@ -1344,30 +1441,30 @@
       <c r="E10" s="3">
         <v>97425</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="32">
         <v>98876</v>
       </c>
       <c r="G10" s="3">
         <v>97625</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="32">
         <v>98256</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="53">
         <v>97179</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="53">
         <v>98050</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="2">
         <v>97433</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="32">
         <v>97441</v>
       </c>
       <c r="D11" s="2">
@@ -1376,30 +1473,30 @@
       <c r="E11" s="3">
         <v>97605</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="32">
         <v>99001</v>
       </c>
       <c r="G11" s="3">
         <v>97306</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="32">
         <v>98221</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="53">
         <v>97418</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="53">
         <v>98217</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="2">
         <v>10624</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="32">
         <v>1784</v>
       </c>
       <c r="D12" s="2">
@@ -1408,138 +1505,138 @@
       <c r="E12" s="3">
         <v>4798</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="32" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="32">
         <v>3004</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="53" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="116"/>
+      <c r="H18" s="116"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="116"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="34" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="35"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="40" t="s">
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="45"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="45"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="48"/>
     </row>
     <row r="21" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="49" t="s">
+      <c r="E21" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="52" t="s">
+      <c r="F21" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="46" t="s">
+      <c r="G21" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="49" t="s">
+      <c r="H21" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="I21" s="52" t="s">
+      <c r="I21" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="46" t="s">
+      <c r="J21" s="54" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="47"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="48"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="2">
         <v>96060</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="32">
         <v>96606</v>
       </c>
       <c r="D24" s="2">
         <v>95636</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="32" t="s">
         <v>30</v>
       </c>
       <c r="F24" s="3">
@@ -1548,30 +1645,30 @@
       <c r="G24" s="3">
         <v>96083</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="I24" s="16" t="s">
+      <c r="I24" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="53" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="2">
         <v>95958</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="32">
         <v>96471</v>
       </c>
       <c r="D25" s="2">
         <v>95464</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="32">
         <v>96310</v>
       </c>
       <c r="F25" s="3">
@@ -1580,30 +1677,30 @@
       <c r="G25" s="3">
         <v>95918</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="53">
         <v>95871</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="32">
         <v>96067</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="53">
         <v>95818</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="2">
         <v>96064</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="32">
         <v>96554</v>
       </c>
       <c r="D26" s="2">
         <v>95740</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="32">
         <v>96371</v>
       </c>
       <c r="F26" s="3">
@@ -1612,30 +1709,30 @@
       <c r="G26" s="3">
         <v>95960</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="53">
         <v>96066</v>
       </c>
-      <c r="I26" s="16">
+      <c r="I26" s="32">
         <v>96346</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="53">
         <v>95957</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="2">
         <v>96218</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="32">
         <v>96667</v>
       </c>
       <c r="D27" s="2">
         <v>95545</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="32">
         <v>96773</v>
       </c>
       <c r="F27" s="3">
@@ -1644,30 +1741,30 @@
       <c r="G27" s="3">
         <v>96437</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="53">
         <v>96184</v>
       </c>
-      <c r="I27" s="16">
+      <c r="I27" s="32">
         <v>96273</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="53">
         <v>96141</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="2">
         <v>1337</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="32" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="32" t="s">
         <v>31</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -1676,165 +1773,165 @@
       <c r="G28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="I28" s="16" t="s">
+      <c r="I28" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="53" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
+      <c r="B33" s="116"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="116"/>
+      <c r="F33" s="116"/>
+      <c r="G33" s="116"/>
+      <c r="H33" s="116"/>
+      <c r="I33" s="116"/>
+      <c r="J33" s="116"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="34" t="s">
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="35"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="40" t="s">
+      <c r="F34" s="27"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I34" s="41"/>
-      <c r="J34" s="42"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="45"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="45"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="48"/>
     </row>
     <row r="36" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="46" t="s">
+      <c r="D36" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="52" t="s">
+      <c r="F36" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="G36" s="46" t="s">
+      <c r="G36" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="H36" s="49" t="s">
+      <c r="H36" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="I36" s="52" t="s">
+      <c r="I36" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="J36" s="46" t="s">
+      <c r="J36" s="54" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="56"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="47"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="56"/>
-      <c r="B38" s="51"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="51"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="48"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="56"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="56"/>
-      <c r="B39" s="49" t="s">
+      <c r="A39" s="18"/>
+      <c r="B39" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="52" t="s">
+      <c r="C39" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="46" t="s">
+      <c r="D39" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="49" t="s">
+      <c r="E39" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="52" t="s">
+      <c r="F39" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="46" t="s">
+      <c r="G39" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="H39" s="49" t="s">
+      <c r="H39" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="I39" s="52" t="s">
+      <c r="I39" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="J39" s="46" t="s">
+      <c r="J39" s="54" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="56"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="47"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="55"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="55"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="32">
         <v>98121</v>
       </c>
       <c r="C41" s="2">
@@ -1849,24 +1946,24 @@
       <c r="F41" s="3">
         <v>97416</v>
       </c>
-      <c r="G41" s="16">
+      <c r="G41" s="32">
         <v>98333</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H41" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="I41" s="16" t="s">
+      <c r="I41" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="J41" s="53" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="32">
         <v>98088</v>
       </c>
       <c r="C42" s="2">
@@ -1881,24 +1978,24 @@
       <c r="F42" s="3">
         <v>97330</v>
       </c>
-      <c r="G42" s="16">
+      <c r="G42" s="32">
         <v>98287</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42" s="53">
         <v>97846</v>
       </c>
-      <c r="I42" s="16">
+      <c r="I42" s="32">
         <v>98341</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="53">
         <v>97496</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="16">
+      <c r="B43" s="32">
         <v>98080</v>
       </c>
       <c r="C43" s="2">
@@ -1913,24 +2010,24 @@
       <c r="F43" s="3">
         <v>97509</v>
       </c>
-      <c r="G43" s="16">
+      <c r="G43" s="32">
         <v>98396</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="53">
         <v>97843</v>
       </c>
-      <c r="I43" s="16">
+      <c r="I43" s="32">
         <v>98488</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="53">
         <v>97471</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="16">
+      <c r="B44" s="32">
         <v>98204</v>
       </c>
       <c r="C44" s="2">
@@ -1945,24 +2042,24 @@
       <c r="F44" s="3">
         <v>97431</v>
       </c>
-      <c r="G44" s="16">
+      <c r="G44" s="32">
         <v>98347</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="53">
         <v>98172</v>
       </c>
-      <c r="I44" s="16">
+      <c r="I44" s="32">
         <v>98390</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44" s="53">
         <v>97876</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="32" t="s">
         <v>46</v>
       </c>
       <c r="C45" s="2">
@@ -1977,328 +2074,351 @@
       <c r="F45" s="3">
         <v>17760</v>
       </c>
-      <c r="G45" s="16">
+      <c r="G45" s="32">
         <v>32569</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H45" s="53">
         <v>7027</v>
       </c>
-      <c r="I45" s="16">
+      <c r="I45" s="32">
         <v>16923</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45" s="53">
         <v>30551</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="59"/>
+      <c r="B49" s="113"/>
+      <c r="C49" s="113"/>
+      <c r="D49" s="113"/>
+      <c r="E49" s="113"/>
+      <c r="F49" s="113"/>
+      <c r="G49" s="113"/>
+      <c r="H49" s="113"/>
+      <c r="I49" s="113"/>
+      <c r="J49" s="114"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="60" t="s">
+      <c r="A50" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="62" t="s">
+      <c r="B50" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="63"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="68" t="s">
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="69"/>
-      <c r="G50" s="70"/>
-      <c r="H50" s="74" t="s">
+      <c r="F50" s="83"/>
+      <c r="G50" s="84"/>
+      <c r="H50" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="I50" s="75"/>
-      <c r="J50" s="76"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="65"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="61"/>
-      <c r="B51" s="65"/>
-      <c r="C51" s="66"/>
-      <c r="D51" s="67"/>
-      <c r="E51" s="71"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="78"/>
-      <c r="J51" s="79"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="85"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="87"/>
+      <c r="H51" s="66"/>
+      <c r="I51" s="67"/>
+      <c r="J51" s="68"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="60" t="s">
+      <c r="A52" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B52" s="81" t="s">
+      <c r="B52" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="84" t="s">
+      <c r="C52" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="87" t="s">
+      <c r="D52" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="E52" s="81" t="s">
+      <c r="E52" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="F52" s="84" t="s">
+      <c r="F52" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="G52" s="87" t="s">
+      <c r="G52" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="H52" s="81" t="s">
+      <c r="H52" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="I52" s="84" t="s">
+      <c r="I52" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="J52" s="87" t="s">
+      <c r="J52" s="71" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="80"/>
-      <c r="B53" s="82"/>
-      <c r="C53" s="85"/>
-      <c r="D53" s="88"/>
-      <c r="E53" s="82"/>
-      <c r="F53" s="85"/>
-      <c r="G53" s="88"/>
-      <c r="H53" s="82"/>
-      <c r="I53" s="85"/>
-      <c r="J53" s="88"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="103"/>
+      <c r="C53" s="104"/>
+      <c r="D53" s="105"/>
+      <c r="E53" s="91"/>
+      <c r="F53" s="92"/>
+      <c r="G53" s="93"/>
+      <c r="H53" s="72"/>
+      <c r="I53" s="73"/>
+      <c r="J53" s="74"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="80"/>
-      <c r="B54" s="83"/>
-      <c r="C54" s="86"/>
-      <c r="D54" s="89"/>
-      <c r="E54" s="83"/>
-      <c r="F54" s="86"/>
-      <c r="G54" s="89"/>
-      <c r="H54" s="83"/>
-      <c r="I54" s="86"/>
-      <c r="J54" s="89"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="106"/>
+      <c r="C54" s="107"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="94"/>
+      <c r="F54" s="95"/>
+      <c r="G54" s="96"/>
+      <c r="H54" s="75"/>
+      <c r="I54" s="76"/>
+      <c r="J54" s="77"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="61"/>
-      <c r="B55" s="9" t="s">
+      <c r="A55" s="10"/>
+      <c r="B55" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="110" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D55" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E55" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="F55" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G55" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="H55" s="9" t="s">
+      <c r="H55" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="I55" s="10" t="s">
+      <c r="I55" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="J55" s="11" t="s">
+      <c r="J55" s="80" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="13">
+      <c r="B56" s="6">
         <v>96602</v>
       </c>
-      <c r="C56" s="13">
+      <c r="C56" s="6">
         <v>96759</v>
       </c>
-      <c r="D56" s="17">
+      <c r="D56" s="33">
         <v>96795</v>
       </c>
-      <c r="E56" s="14">
+      <c r="E56" s="7">
         <v>97129</v>
       </c>
-      <c r="F56" s="14">
+      <c r="F56" s="7">
         <v>97193</v>
       </c>
-      <c r="G56" s="18">
+      <c r="G56" s="34">
         <v>97274</v>
       </c>
-      <c r="H56" s="15">
+      <c r="H56" s="81">
         <v>97191</v>
       </c>
-      <c r="I56" s="17">
+      <c r="I56" s="33">
         <v>97717</v>
       </c>
-      <c r="J56" s="15">
+      <c r="J56" s="81">
         <v>97434</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B57" s="13">
+      <c r="B57" s="6">
         <v>96568</v>
       </c>
-      <c r="C57" s="13">
+      <c r="C57" s="6">
         <v>96847</v>
       </c>
-      <c r="D57" s="17">
+      <c r="D57" s="33">
         <v>96819</v>
       </c>
-      <c r="E57" s="14">
+      <c r="E57" s="7">
         <v>97153</v>
       </c>
-      <c r="F57" s="14">
+      <c r="F57" s="7">
         <v>97274</v>
       </c>
-      <c r="G57" s="18">
+      <c r="G57" s="34">
         <v>97337</v>
       </c>
-      <c r="H57" s="15">
+      <c r="H57" s="81">
         <v>97264</v>
       </c>
-      <c r="I57" s="17">
+      <c r="I57" s="33">
         <v>97722</v>
       </c>
-      <c r="J57" s="15">
+      <c r="J57" s="81">
         <v>97494</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="13">
+      <c r="B58" s="6">
         <v>97393</v>
       </c>
-      <c r="C58" s="13">
+      <c r="C58" s="6">
         <v>97524</v>
       </c>
-      <c r="D58" s="17">
+      <c r="D58" s="33">
         <v>97490</v>
       </c>
-      <c r="E58" s="14">
+      <c r="E58" s="7">
         <v>97824</v>
       </c>
-      <c r="F58" s="14">
+      <c r="F58" s="7">
         <v>97954</v>
       </c>
-      <c r="G58" s="18">
+      <c r="G58" s="34">
         <v>98131</v>
       </c>
-      <c r="H58" s="15">
+      <c r="H58" s="81">
         <v>98596</v>
       </c>
-      <c r="I58" s="17">
+      <c r="I58" s="33">
         <v>98625</v>
       </c>
-      <c r="J58" s="15">
+      <c r="J58" s="81">
         <v>98335</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="13">
+      <c r="B59" s="6">
         <v>95812</v>
       </c>
-      <c r="C59" s="13">
+      <c r="C59" s="6">
         <v>96227</v>
       </c>
-      <c r="D59" s="17">
+      <c r="D59" s="33">
         <v>96188</v>
       </c>
-      <c r="E59" s="14">
+      <c r="E59" s="7">
         <v>96557</v>
       </c>
-      <c r="F59" s="14">
+      <c r="F59" s="7">
         <v>96647</v>
       </c>
-      <c r="G59" s="18">
+      <c r="G59" s="34">
         <v>96605</v>
       </c>
-      <c r="H59" s="15">
+      <c r="H59" s="81">
         <v>96008</v>
       </c>
-      <c r="I59" s="17">
+      <c r="I59" s="33">
         <v>96889</v>
       </c>
-      <c r="J59" s="15">
+      <c r="J59" s="81">
         <v>96724</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="13">
+      <c r="B60" s="6">
         <v>183929</v>
       </c>
-      <c r="C60" s="13">
+      <c r="C60" s="6">
         <v>254667</v>
       </c>
-      <c r="D60" s="17">
+      <c r="D60" s="33">
         <v>276158</v>
       </c>
-      <c r="E60" s="14">
+      <c r="E60" s="7">
         <v>165595</v>
       </c>
-      <c r="F60" s="14">
+      <c r="F60" s="7">
         <v>233255</v>
       </c>
-      <c r="G60" s="18">
+      <c r="G60" s="34">
         <v>246635</v>
       </c>
-      <c r="H60" s="15">
+      <c r="H60" s="81">
         <v>140410</v>
       </c>
-      <c r="I60" s="17">
+      <c r="I60" s="33">
         <v>215629</v>
       </c>
-      <c r="J60" s="15">
+      <c r="J60" s="81">
         <v>268728</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="G52:G54"/>
-    <mergeCell ref="H52:H54"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="J52:J54"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:D51"/>
-    <mergeCell ref="E50:G51"/>
-    <mergeCell ref="H50:J51"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="E3:G4"/>
+    <mergeCell ref="H3:J4"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:D20"/>
+    <mergeCell ref="E19:G20"/>
+    <mergeCell ref="H19:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:D35"/>
+    <mergeCell ref="E34:G35"/>
+    <mergeCell ref="H34:J35"/>
     <mergeCell ref="G39:G40"/>
     <mergeCell ref="H39:H40"/>
     <mergeCell ref="I39:I40"/>
@@ -2315,44 +2435,21 @@
     <mergeCell ref="I36:I38"/>
     <mergeCell ref="J36:J38"/>
     <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:D35"/>
-    <mergeCell ref="E34:G35"/>
-    <mergeCell ref="H34:J35"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="A18:J18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:D20"/>
-    <mergeCell ref="E19:G20"/>
-    <mergeCell ref="H19:J20"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="E3:G4"/>
-    <mergeCell ref="H3:J4"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:D51"/>
+    <mergeCell ref="E50:G51"/>
+    <mergeCell ref="H50:J51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="H52:H54"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="J52:J54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>